<commit_message>
Limpieza datos y Series
</commit_message>
<xml_diff>
--- a/VENTAS-HIDROCARBUROS-2025-05.xlsx
+++ b/VENTAS-HIDROCARBUROS-2025-05.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Base de datos Estadistica\03 Presentación de datos\Web Estadisticas\ESTADISTICAS DE COMERCIALIZACION\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dcuellar\Descarga\lab1DS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD7A666-9D9D-4D43-BDE3-157882BE86AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B10525-FC0C-42ED-8DA2-2325A77F0D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0B398B4E-6917-452C-A48B-BAC57D309DD0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0B398B4E-6917-452C-A48B-BAC57D309DD0}"/>
   </bookViews>
   <sheets>
     <sheet name="VENTAS_IMP" sheetId="1" r:id="rId1"/>
@@ -125,7 +125,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmm/yyyy"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -232,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -259,10 +259,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -275,16 +275,15 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,9 +468,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -509,7 +508,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -615,7 +614,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -757,7 +756,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -774,7 +773,7 @@
       <selection pane="bottomRight" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="15.7109375" style="3" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" style="3" customWidth="1"/>
@@ -797,7 +796,7 @@
     <col min="20" max="16384" width="14.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" ht="15.75">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
@@ -818,7 +817,7 @@
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
     </row>
-    <row r="2" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="15.75">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
@@ -839,7 +838,7 @@
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
     </row>
-    <row r="3" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="15.75">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
@@ -860,7 +859,7 @@
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
     </row>
-    <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" ht="15.75">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="2"/>
@@ -881,7 +880,7 @@
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
     </row>
-    <row r="5" spans="1:19" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" ht="12" customHeight="1">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -902,7 +901,7 @@
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
     </row>
-    <row r="6" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" ht="14.25">
       <c r="A6" s="8" t="s">
         <v>0</v>
       </c>
@@ -925,7 +924,7 @@
       <c r="R6" s="9"/>
       <c r="S6" s="9"/>
     </row>
-    <row r="7" spans="1:19" s="12" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" s="12" customFormat="1" ht="42.75" customHeight="1">
       <c r="A7" s="13" t="s">
         <v>1</v>
       </c>
@@ -984,7 +983,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="19" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" ht="24" customHeight="1">
       <c r="A8" s="16">
         <v>45658</v>
       </c>
@@ -1040,7 +1039,7 @@
         <v>4167063.3700000006</v>
       </c>
     </row>
-    <row r="9" spans="1:19" s="19" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" ht="24" customHeight="1">
       <c r="A9" s="16">
         <v>45689</v>
       </c>
@@ -1100,7 +1099,7 @@
         <v>4130792.38</v>
       </c>
     </row>
-    <row r="10" spans="1:19" s="19" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" ht="24" customHeight="1">
       <c r="A10" s="16">
         <v>45717</v>
       </c>
@@ -1160,7 +1159,7 @@
         <v>4507787.5999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:19" s="19" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" ht="24" customHeight="1">
       <c r="A11" s="16">
         <v>45748</v>
       </c>
@@ -1218,7 +1217,7 @@
         <v>4419979.7300000004</v>
       </c>
     </row>
-    <row r="12" spans="1:19" s="19" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" ht="24" customHeight="1">
       <c r="A12" s="16">
         <v>45778</v>
       </c>
@@ -1274,7 +1273,7 @@
         <v>4517749.8899999997</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" ht="18.75" customHeight="1">
       <c r="A13" s="10"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -1295,12 +1294,12 @@
       <c r="R13" s="11"/>
       <c r="S13" s="11"/>
     </row>
-    <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" ht="15" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" ht="15" customHeight="1">
       <c r="A15" s="3" t="s">
         <v>20</v>
       </c>

</xml_diff>